<commit_message>
float instead of double
</commit_message>
<xml_diff>
--- a/src/main/resources/Data.xlsx
+++ b/src/main/resources/Data.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="example1" sheetId="1" r:id="rId1"/>
-    <sheet name="list" sheetId="4" r:id="rId2"/>
-    <sheet name="emp" sheetId="2" r:id="rId3"/>
-    <sheet name="paycheck" sheetId="5" r:id="rId4"/>
+    <sheet name="employees" sheetId="6" r:id="rId2"/>
+    <sheet name="list" sheetId="4" r:id="rId3"/>
+    <sheet name="emp" sheetId="2" r:id="rId4"/>
+    <sheet name="pay" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="60">
   <si>
     <t>true</t>
   </si>
@@ -51,9 +52,6 @@
     <t>Charkiv</t>
   </si>
   <si>
-    <t>Kuyiv</t>
-  </si>
-  <si>
     <t>Dnipro</t>
   </si>
   <si>
@@ -72,27 +70,9 @@
     <t>Bool**Sunday_off</t>
   </si>
   <si>
-    <t>emp**employees</t>
-  </si>
-  <si>
     <t>list**goods</t>
   </si>
   <si>
-    <t>Employee_1</t>
-  </si>
-  <si>
-    <t>Employee_5</t>
-  </si>
-  <si>
-    <t>Employee_4</t>
-  </si>
-  <si>
-    <t>Employee_3</t>
-  </si>
-  <si>
-    <t>Employee_2</t>
-  </si>
-  <si>
     <t>Wasja</t>
   </si>
   <si>
@@ -132,34 +112,97 @@
     <t>bool**tobacco</t>
   </si>
   <si>
-    <t>val1</t>
-  </si>
-  <si>
-    <t>val2</t>
-  </si>
-  <si>
-    <t>1aaa</t>
-  </si>
-  <si>
-    <t>1bbb</t>
-  </si>
-  <si>
-    <t>2aaa</t>
-  </si>
-  <si>
-    <t>2bbb</t>
-  </si>
-  <si>
-    <t>3aaa</t>
-  </si>
-  <si>
-    <t>3bbb</t>
-  </si>
-  <si>
-    <t>doub**val3</t>
-  </si>
-  <si>
-    <t>arr**paycheck</t>
+    <t>First_Name</t>
+  </si>
+  <si>
+    <t>Last_Name</t>
+  </si>
+  <si>
+    <t>int**Age</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Smith</t>
+  </si>
+  <si>
+    <t>Johnson</t>
+  </si>
+  <si>
+    <t>Williams</t>
+  </si>
+  <si>
+    <t>Brown</t>
+  </si>
+  <si>
+    <t>Davis</t>
+  </si>
+  <si>
+    <t>Miller</t>
+  </si>
+  <si>
+    <t>Wilson</t>
+  </si>
+  <si>
+    <t>Moore</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>int**Id</t>
+  </si>
+  <si>
+    <t>arr**employees</t>
+  </si>
+  <si>
+    <t>emp**emploee0</t>
+  </si>
+  <si>
+    <t>emp**emploee1</t>
+  </si>
+  <si>
+    <t>emp**emploee2</t>
+  </si>
+  <si>
+    <t>emp**emploee3</t>
+  </si>
+  <si>
+    <t>Kyiv</t>
+  </si>
+  <si>
+    <t>&lt;-- point off  row number that's used in list sheet</t>
+  </si>
+  <si>
+    <t>&lt;-- point off  row number that's used in employees sheet</t>
+  </si>
+  <si>
+    <t>&lt;-- point off  row number that's used in emp sheet</t>
+  </si>
+  <si>
+    <t>c**Comment</t>
+  </si>
+  <si>
+    <t>us****user_id</t>
+  </si>
+  <si>
+    <t>row****num</t>
+  </si>
+  <si>
+    <t>pay**paycheck</t>
+  </si>
+  <si>
+    <t>c****comment</t>
+  </si>
+  <si>
+    <t>flo**salary</t>
+  </si>
+  <si>
+    <t>flo**bonus</t>
   </si>
 </sst>
 </file>
@@ -195,10 +238,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -479,50 +523,54 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.28515625" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="17.140625" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" customWidth="1"/>
-    <col min="7" max="7" width="17" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" customWidth="1"/>
+    <col min="4" max="4" width="17" customWidth="1"/>
+    <col min="5" max="5" width="22.5703125" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="17.140625" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" customWidth="1"/>
+    <col min="9" max="9" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>11</v>
+        <v>25</v>
+      </c>
+      <c r="D1" t="s">
+        <v>44</v>
       </c>
       <c r="E1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" t="s">
         <v>15</v>
       </c>
-      <c r="F1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -532,68 +580,68 @@
       <c r="C2">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>12</v>
+      <c r="D2">
+        <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
+        <v>51</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
         <v>0</v>
       </c>
       <c r="H2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>49</v>
       </c>
       <c r="C3">
         <v>3</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F3">
+      <c r="D3">
         <v>1</v>
       </c>
-      <c r="G3">
+      <c r="F3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H3">
         <v>1</v>
       </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4">
         <v>2</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F4">
-        <v>2</v>
-      </c>
-      <c r="G4">
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4">
         <v>2</v>
       </c>
     </row>
@@ -605,82 +653,83 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="15" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" customWidth="1"/>
+    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B1" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="C1" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="D1" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="E1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" t="s">
-        <v>2</v>
+        <v>47</v>
+      </c>
+      <c r="F1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="G2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>7</v>
+      </c>
+      <c r="D3">
+        <v>6</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -690,67 +739,98 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" customWidth="1"/>
-    <col min="2" max="3" width="14.42578125" customWidth="1"/>
-    <col min="4" max="4" width="16" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>55</v>
       </c>
       <c r="B1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="F1" t="s">
         <v>23</v>
       </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
       <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>24</v>
-      </c>
       <c r="B3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>27</v>
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -759,56 +839,277 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.7109375" customWidth="1"/>
+    <col min="3" max="4" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2">
+        <v>19</v>
+      </c>
+      <c r="E2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3">
+        <v>25</v>
+      </c>
+      <c r="E3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="1">
+        <v>42</v>
+      </c>
+      <c r="E4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="1">
+        <v>19</v>
+      </c>
+      <c r="E5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" s="1">
+        <v>18</v>
+      </c>
+      <c r="E6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="1">
+        <v>25</v>
+      </c>
+      <c r="E7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="1">
+        <v>21</v>
+      </c>
+      <c r="E8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="1">
+        <v>20</v>
+      </c>
+      <c r="E9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" customWidth="1"/>
+    <col min="2" max="3" width="14.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="B1" t="s">
-        <v>37</v>
+        <v>58</v>
       </c>
       <c r="C1" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2">
-        <v>0.56899999999999995</v>
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B3" t="s">
-        <v>41</v>
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>25</v>
       </c>
       <c r="C3">
-        <v>666</v>
+        <v>4.75</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B4" t="s">
-        <v>43</v>
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>22</v>
       </c>
       <c r="C4">
-        <v>12</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>33.299999999999997</v>
+      </c>
+      <c r="C5">
+        <v>5.8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>